<commit_message>
Formato de fechas para calculo de dias trabajados durante el contrato
</commit_message>
<xml_diff>
--- a/Base para desarrollo de liquidacion empleados.xlsx
+++ b/Base para desarrollo de liquidacion empleados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigjh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Documents\Python\004. Liquidacion de empleados\Liquidacion_de_empleados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50D5A12D-ACBF-4C43-BBD8-684842E58176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5175D121-F71C-4CFF-90C8-6F3B2A414B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liquidación" sheetId="1" r:id="rId1"/>
@@ -1419,6 +1419,46 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="27" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="24" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="24" fillId="0" borderId="15" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="24" fillId="0" borderId="17" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="34" fillId="25" borderId="10" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="34" fillId="25" borderId="12" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="13" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="34" fillId="25" borderId="11" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
@@ -1427,15 +1467,6 @@
     </xf>
     <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="34" fillId="25" borderId="10" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="34" fillId="25" borderId="11" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="34" fillId="25" borderId="12" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1462,37 +1493,6 @@
     <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="15" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="17" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="15" fontId="27" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="15" fontId="24" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="13" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1513,54 +1513,54 @@
     </xf>
   </cellXfs>
   <cellStyles count="48">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="24" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="25" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="27" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="28" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="29" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="31" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="20" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="21" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="42" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="19" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="46" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="23" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="30" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="22" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="19" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="20" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="21" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="22" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="23" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="24" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="25" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="27" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="28" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="29" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="30" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="31" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Millares 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Millares 2_Libro1(1)" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="Neutral" xfId="34" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_1299 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="Normal_1299 2_Libro1(1)" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="38" builtinId="5"/>
+    <cellStyle name="Notas" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Porcentaje" xfId="38" builtinId="5"/>
     <cellStyle name="Porcentual 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Title" xfId="43" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="40" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="42" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="43" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 1" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Título 2" xfId="45" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="46" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="47" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1843,69 +1843,69 @@
   </sheetPr>
   <dimension ref="B1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:F46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="113" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" style="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="113" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="113" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="113" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="113" customWidth="1"/>
     <col min="4" max="4" width="8" style="113" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="113" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.88671875" style="113" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="113" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="113" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" style="113" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="113" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" style="113" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="113" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="113" customWidth="1"/>
     <col min="10" max="10" width="14" style="113" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" style="113" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="113" customWidth="1"/>
     <col min="12" max="12" width="9" style="113" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="113"/>
+    <col min="13" max="16384" width="11.42578125" style="113"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="161" t="s">
+    <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="142" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161"/>
-      <c r="J2" s="161"/>
-    </row>
-    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="161" t="s">
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+    </row>
+    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="142" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-    </row>
-    <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="162" t="s">
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+    </row>
+    <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="143" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="162"/>
-      <c r="G4" s="162"/>
-      <c r="H4" s="162"/>
-      <c r="I4" s="162"/>
-      <c r="J4" s="162"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
       <c r="K4" s="114"/>
     </row>
-    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="74"/>
       <c r="C5" s="74"/>
       <c r="D5" s="74"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="K5" s="114"/>
     </row>
-    <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1930,67 +1930,67 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="160" t="s">
+      <c r="C7" s="152" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="160"/>
-      <c r="E7" s="160"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="160"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="152"/>
+      <c r="F7" s="152"/>
+      <c r="G7" s="152"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="163" t="s">
+      <c r="C8" s="144" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
+      <c r="D8" s="144"/>
+      <c r="E8" s="144"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="159" t="s">
+      <c r="C9" s="153" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="159"/>
-      <c r="E9" s="159"/>
+      <c r="D9" s="153"/>
+      <c r="E9" s="153"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="160" t="s">
+      <c r="C10" s="152" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="160"/>
-      <c r="E10" s="160"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="152"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="4"/>
       <c r="D11" s="3"/>
@@ -2001,7 +2001,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2012,27 +2012,27 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="145" t="s">
+    <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="147" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="147"/>
+      <c r="C13" s="148"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="145" t="s">
+      <c r="E13" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="147"/>
-    </row>
-    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="151"/>
+      <c r="G13" s="151"/>
+      <c r="H13" s="151"/>
+      <c r="I13" s="151"/>
+      <c r="J13" s="148"/>
+    </row>
+    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="75" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="67">
-        <v>44129</v>
+        <v>45078</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7" t="s">
@@ -2042,10 +2042,10 @@
       <c r="H14" s="8"/>
       <c r="I14" s="9"/>
       <c r="J14" s="68">
-        <v>1350000</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="75" t="s">
         <v>3</v>
       </c>
@@ -2060,16 +2060,16 @@
       <c r="H15" s="8"/>
       <c r="I15" s="9"/>
       <c r="J15" s="68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="75" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="77">
         <f>DAYS360(C15,C14)+1</f>
-        <v>742</v>
+        <v>1678</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="7" t="s">
@@ -2083,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B17" s="39" t="s">
         <v>83</v>
       </c>
@@ -2101,15 +2101,15 @@
       <c r="I17" s="41"/>
       <c r="J17" s="56">
         <f>IF(SUM(J15:J16)&gt;SUM(J14:J15),SUM(J15:J16),SUM(J14:J15))</f>
-        <v>1350000</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2650000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
         <v>63</v>
       </c>
       <c r="C18" s="78">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="36" t="s">
@@ -2123,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="86"/>
       <c r="C19" s="11"/>
       <c r="D19" s="3"/>
@@ -2134,81 +2134,81 @@
       <c r="I19" s="13"/>
       <c r="J19" s="85"/>
     </row>
-    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="145" t="s">
+    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="147"/>
+      <c r="C20" s="148"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="145" t="s">
+      <c r="E20" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="146"/>
-      <c r="G20" s="146"/>
-      <c r="H20" s="146"/>
-      <c r="I20" s="146"/>
-      <c r="J20" s="147"/>
-    </row>
-    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="151"/>
+      <c r="J20" s="148"/>
+    </row>
+    <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="75" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="67">
-        <v>41937</v>
+        <v>44932</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="164" t="s">
+      <c r="E21" s="149" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="158"/>
-      <c r="G21" s="158"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="158"/>
+      <c r="F21" s="150"/>
+      <c r="G21" s="150"/>
+      <c r="H21" s="150"/>
+      <c r="I21" s="150"/>
       <c r="J21" s="67">
         <v>44129</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="75" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="67">
-        <v>41916</v>
+        <v>44927</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="164" t="s">
+      <c r="E22" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
-      <c r="H22" s="158"/>
-      <c r="I22" s="158"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
+      <c r="H22" s="150"/>
+      <c r="I22" s="150"/>
       <c r="J22" s="67">
         <v>44108</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="42" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="43">
         <f>DAYS360(C22,C21)+1</f>
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="156" t="s">
+      <c r="E23" s="145" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="157"/>
-      <c r="G23" s="157"/>
-      <c r="H23" s="157"/>
-      <c r="I23" s="157"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="146"/>
+      <c r="H23" s="146"/>
+      <c r="I23" s="146"/>
       <c r="J23" s="43">
         <f>DAYS360(J22,J21)+1</f>
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="86"/>
       <c r="C24" s="11"/>
       <c r="D24" s="3"/>
@@ -2219,86 +2219,86 @@
       <c r="I24" s="9"/>
       <c r="J24" s="84"/>
     </row>
-    <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="145" t="s">
+    <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="147"/>
+      <c r="C25" s="148"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="145" t="s">
+      <c r="E25" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="146"/>
-      <c r="I25" s="146"/>
-      <c r="J25" s="147"/>
-    </row>
-    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="151"/>
+      <c r="G25" s="151"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="151"/>
+      <c r="J25" s="148"/>
+    </row>
+    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="75" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="67">
-        <v>41937</v>
+        <v>44933</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="164" t="s">
+      <c r="E26" s="149" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="158"/>
-      <c r="G26" s="158"/>
-      <c r="H26" s="158"/>
-      <c r="I26" s="158"/>
+      <c r="F26" s="150"/>
+      <c r="G26" s="150"/>
+      <c r="H26" s="150"/>
+      <c r="I26" s="150"/>
       <c r="J26" s="67">
         <v>44129</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="75" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="67">
-        <v>41916</v>
+        <v>39980</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="164" t="s">
+      <c r="E27" s="149" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="158"/>
-      <c r="G27" s="158"/>
-      <c r="H27" s="158"/>
-      <c r="I27" s="158"/>
+      <c r="F27" s="150"/>
+      <c r="G27" s="150"/>
+      <c r="H27" s="150"/>
+      <c r="I27" s="150"/>
       <c r="J27" s="67">
         <v>44108</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="75" t="s">
         <v>73</v>
       </c>
       <c r="C28" s="29">
         <f>((DAYS360(C27,C26)+1)*15)/360</f>
-        <v>0.91666666666666663</v>
+        <v>203.41666666666666</v>
       </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="156" t="s">
+      <c r="E28" s="145" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="146"/>
+      <c r="I28" s="146"/>
       <c r="J28" s="43">
         <f>DAYS360(J27,J26)+1</f>
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="75" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="71">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -2308,23 +2308,23 @@
       <c r="I29" s="9"/>
       <c r="J29" s="84"/>
     </row>
-    <row r="30" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="42" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="43">
         <f>+C28-C29</f>
-        <v>0.91666666666666663</v>
+        <v>8.4166666666666572</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="158"/>
-      <c r="F30" s="158"/>
-      <c r="G30" s="158"/>
-      <c r="H30" s="158"/>
-      <c r="I30" s="158"/>
+      <c r="E30" s="150"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="150"/>
+      <c r="H30" s="150"/>
+      <c r="I30" s="150"/>
       <c r="J30" s="16"/>
     </row>
-    <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="86"/>
       <c r="C31" s="11"/>
       <c r="D31" s="3"/>
@@ -2335,43 +2335,43 @@
       <c r="I31" s="9"/>
       <c r="J31" s="84"/>
     </row>
-    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="145" t="s">
+    <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="147" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="146"/>
-      <c r="D32" s="146"/>
-      <c r="E32" s="146"/>
-      <c r="F32" s="146"/>
-      <c r="G32" s="146"/>
-      <c r="H32" s="146"/>
-      <c r="I32" s="146"/>
-      <c r="J32" s="147"/>
-    </row>
-    <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="151"/>
+      <c r="D32" s="151"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="151"/>
+      <c r="G32" s="151"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="151"/>
+      <c r="J32" s="148"/>
+    </row>
+    <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="155" t="s">
+      <c r="C33" s="164" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="155"/>
-      <c r="E33" s="155"/>
-      <c r="F33" s="155"/>
-      <c r="G33" s="155"/>
-      <c r="H33" s="155"/>
-      <c r="I33" s="155"/>
+      <c r="D33" s="164"/>
+      <c r="E33" s="164"/>
+      <c r="F33" s="164"/>
+      <c r="G33" s="164"/>
+      <c r="H33" s="164"/>
+      <c r="I33" s="164"/>
       <c r="J33" s="26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C34" s="19">
         <f>J17-J15</f>
-        <v>1350000</v>
+        <v>2500000</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>8</v>
@@ -2384,22 +2384,22 @@
       </c>
       <c r="G34" s="3">
         <f>C30</f>
-        <v>0.91666666666666663</v>
+        <v>8.4166666666666572</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="17">
         <f>((C34/E34)*G34)</f>
-        <v>41250</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>701388.88888888806</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C35" s="19">
         <f>J17</f>
-        <v>1350000</v>
+        <v>2650000</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>8</v>
@@ -2420,16 +2420,16 @@
       <c r="I35" s="18"/>
       <c r="J35" s="17">
         <f t="shared" ref="J35:J41" si="0">((C35/E35)*G35)</f>
-        <v>82500</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>161944.44444444444</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C36" s="19">
         <f>$J$35</f>
-        <v>82500</v>
+        <v>161944.44444444444</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>8</v>
@@ -2452,16 +2452,16 @@
       </c>
       <c r="J36" s="17">
         <f>(((C36/E36)*G36)*I36)</f>
-        <v>604.99999999999989</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1187.5925925925926</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="19">
         <f>J17</f>
-        <v>1350000</v>
+        <v>2650000</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>8</v>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="G37" s="10">
         <f>C23</f>
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>9</v>
@@ -2482,16 +2482,16 @@
       <c r="I37" s="18"/>
       <c r="J37" s="17">
         <f t="shared" si="0"/>
-        <v>82500</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>44166.666666666672</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="19">
         <f>J14</f>
-        <v>1350000</v>
+        <v>2500000</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>8</v>
@@ -2504,17 +2504,17 @@
       </c>
       <c r="G38" s="3">
         <f>C18</f>
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="18"/>
       <c r="J38" s="17">
         <f t="shared" si="0"/>
-        <v>990000</v>
+        <v>500000</v>
       </c>
       <c r="M38" s="117"/>
     </row>
-    <row r="39" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
         <v>12</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
         <v>46</v>
       </c>
@@ -2548,13 +2548,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="19">
         <f>J15</f>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>8</v>
@@ -2567,32 +2567,32 @@
       </c>
       <c r="G41" s="3">
         <f>C18</f>
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="44">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="156" t="s">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="145" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="157"/>
-      <c r="D42" s="157"/>
-      <c r="E42" s="157"/>
-      <c r="F42" s="157"/>
-      <c r="G42" s="157"/>
-      <c r="H42" s="157"/>
-      <c r="I42" s="157"/>
+      <c r="C42" s="146"/>
+      <c r="D42" s="146"/>
+      <c r="E42" s="146"/>
+      <c r="F42" s="146"/>
+      <c r="G42" s="146"/>
+      <c r="H42" s="146"/>
+      <c r="I42" s="146"/>
       <c r="J42" s="40">
         <f>SUM(J34:J41)</f>
-        <v>1196855</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>1438687.5925925919</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
@@ -2603,20 +2603,20 @@
       <c r="I43" s="22"/>
       <c r="J43" s="87"/>
     </row>
-    <row r="44" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="145" t="s">
+    <row r="44" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="146"/>
-      <c r="D44" s="146"/>
-      <c r="E44" s="146"/>
-      <c r="F44" s="146"/>
-      <c r="G44" s="146"/>
-      <c r="H44" s="146"/>
-      <c r="I44" s="146"/>
-      <c r="J44" s="147"/>
-    </row>
-    <row r="45" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="151"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="151"/>
+      <c r="F44" s="151"/>
+      <c r="G44" s="151"/>
+      <c r="H44" s="151"/>
+      <c r="I44" s="151"/>
+      <c r="J44" s="148"/>
+    </row>
+    <row r="45" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="50" t="s">
         <v>75</v>
       </c>
@@ -2624,18 +2624,18 @@
         <v>79</v>
       </c>
       <c r="D45" s="76"/>
-      <c r="E45" s="148" t="s">
+      <c r="E45" s="157" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="148"/>
-      <c r="G45" s="148"/>
+      <c r="F45" s="157"/>
+      <c r="G45" s="157"/>
       <c r="H45" s="48"/>
       <c r="I45" s="49"/>
       <c r="J45" s="51" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
         <v>14</v>
       </c>
@@ -2643,20 +2643,20 @@
         <v>0.04</v>
       </c>
       <c r="D46" s="15"/>
-      <c r="E46" s="149">
+      <c r="E46" s="158">
         <f>IF($J$38&lt;0,$J$34+$J$39,$J$38+$J$39+$J$34)</f>
-        <v>1031250</v>
-      </c>
-      <c r="F46" s="149"/>
+        <v>1201388.8888888881</v>
+      </c>
+      <c r="F46" s="158"/>
       <c r="G46" s="21"/>
       <c r="H46" s="19"/>
       <c r="I46" s="21"/>
       <c r="J46" s="52">
         <f>(SUM(E46:G46)*-C46)</f>
-        <v>-41250</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>-48055.555555555526</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
         <v>68</v>
       </c>
@@ -2664,27 +2664,27 @@
         <v>0.04</v>
       </c>
       <c r="D47" s="15"/>
-      <c r="E47" s="149">
+      <c r="E47" s="158">
         <f>IF($J$38&lt;0,$J$34+$J$39,$J$38+$J$39+$J$34)</f>
-        <v>1031250</v>
-      </c>
-      <c r="F47" s="149"/>
+        <v>1201388.8888888881</v>
+      </c>
+      <c r="F47" s="158"/>
       <c r="G47" s="45"/>
       <c r="H47" s="19"/>
       <c r="I47" s="21"/>
       <c r="J47" s="52">
         <f>(SUM(E47:G47)*-C47)</f>
-        <v>-41250</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-48055.555555555526</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="46"/>
-      <c r="E48" s="154"/>
-      <c r="F48" s="154"/>
+      <c r="E48" s="163"/>
+      <c r="F48" s="163"/>
       <c r="G48" s="21"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -2692,24 +2692,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="156" t="s">
+    <row r="49" spans="2:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="145" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="157"/>
-      <c r="D49" s="157"/>
-      <c r="E49" s="157"/>
-      <c r="F49" s="157"/>
-      <c r="G49" s="157"/>
-      <c r="H49" s="157"/>
-      <c r="I49" s="157"/>
+      <c r="C49" s="146"/>
+      <c r="D49" s="146"/>
+      <c r="E49" s="146"/>
+      <c r="F49" s="146"/>
+      <c r="G49" s="146"/>
+      <c r="H49" s="146"/>
+      <c r="I49" s="146"/>
       <c r="J49" s="53">
         <f>SUM(J46:J48)</f>
-        <v>-82500</v>
+        <v>-96111.111111111051</v>
       </c>
       <c r="K49" s="118"/>
     </row>
-    <row r="50" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="24"/>
       <c r="C50" s="14"/>
       <c r="D50" s="22"/>
@@ -2721,7 +2721,7 @@
       <c r="J50" s="87"/>
       <c r="K50" s="118"/>
     </row>
-    <row r="51" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="35" t="s">
         <v>69</v>
       </c>
@@ -2734,11 +2734,11 @@
       <c r="I51" s="59"/>
       <c r="J51" s="61">
         <f>+J42+J49</f>
-        <v>1114355</v>
+        <v>1342576.4814814809</v>
       </c>
       <c r="K51" s="118"/>
     </row>
-    <row r="52" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="C52" s="14"/>
       <c r="D52" s="22"/>
@@ -2750,36 +2750,36 @@
       <c r="J52" s="54"/>
       <c r="K52" s="118"/>
     </row>
-    <row r="53" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="150" t="str">
+      <c r="C53" s="159" t="str">
         <f>'Conversor numeros letras'!B2</f>
-        <v>UN MILLÓN CIENTO CATORCE MIL TRESCIENTOS CINCUENTA Y CINCO PESOS M/C</v>
-      </c>
-      <c r="D53" s="150"/>
-      <c r="E53" s="150"/>
-      <c r="F53" s="150"/>
-      <c r="G53" s="150"/>
-      <c r="H53" s="150"/>
-      <c r="I53" s="150"/>
-      <c r="J53" s="151"/>
+        <v>UN MILLÓN TRESCIENTOS CUARENTA Y DOS MIL QUINIENTOS SETENTA Y SEIS PESOS M/C</v>
+      </c>
+      <c r="D53" s="159"/>
+      <c r="E53" s="159"/>
+      <c r="F53" s="159"/>
+      <c r="G53" s="159"/>
+      <c r="H53" s="159"/>
+      <c r="I53" s="159"/>
+      <c r="J53" s="160"/>
       <c r="K53" s="118"/>
     </row>
-    <row r="54" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="27"/>
-      <c r="C54" s="152"/>
-      <c r="D54" s="152"/>
-      <c r="E54" s="152"/>
-      <c r="F54" s="152"/>
-      <c r="G54" s="152"/>
-      <c r="H54" s="152"/>
-      <c r="I54" s="152"/>
-      <c r="J54" s="153"/>
+      <c r="C54" s="161"/>
+      <c r="D54" s="161"/>
+      <c r="E54" s="161"/>
+      <c r="F54" s="161"/>
+      <c r="G54" s="161"/>
+      <c r="H54" s="161"/>
+      <c r="I54" s="161"/>
+      <c r="J54" s="162"/>
       <c r="K54" s="118"/>
     </row>
-    <row r="55" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="28"/>
@@ -2791,7 +2791,7 @@
       <c r="J55" s="28"/>
       <c r="K55" s="119"/>
     </row>
-    <row r="56" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="22" t="s">
         <v>17</v>
       </c>
@@ -2805,102 +2805,102 @@
       <c r="J56" s="46"/>
       <c r="K56" s="119"/>
     </row>
-    <row r="57" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="143" t="s">
+    <row r="57" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="155" t="s">
         <v>106</v>
       </c>
-      <c r="C57" s="143"/>
-      <c r="D57" s="143"/>
-      <c r="E57" s="143"/>
-      <c r="F57" s="143"/>
-      <c r="G57" s="143"/>
-      <c r="H57" s="143"/>
-      <c r="I57" s="143"/>
-      <c r="J57" s="143"/>
+      <c r="C57" s="155"/>
+      <c r="D57" s="155"/>
+      <c r="E57" s="155"/>
+      <c r="F57" s="155"/>
+      <c r="G57" s="155"/>
+      <c r="H57" s="155"/>
+      <c r="I57" s="155"/>
+      <c r="J57" s="155"/>
       <c r="K57" s="119"/>
     </row>
-    <row r="58" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="143"/>
-      <c r="C58" s="143"/>
-      <c r="D58" s="143"/>
-      <c r="E58" s="143"/>
-      <c r="F58" s="143"/>
-      <c r="G58" s="143"/>
-      <c r="H58" s="143"/>
-      <c r="I58" s="143"/>
-      <c r="J58" s="143"/>
-    </row>
-    <row r="59" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="143"/>
-      <c r="C59" s="143"/>
-      <c r="D59" s="143"/>
-      <c r="E59" s="143"/>
-      <c r="F59" s="143"/>
-      <c r="G59" s="143"/>
-      <c r="H59" s="143"/>
-      <c r="I59" s="143"/>
-      <c r="J59" s="143"/>
-    </row>
-    <row r="60" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="144" t="str">
+    <row r="58" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="155"/>
+      <c r="C58" s="155"/>
+      <c r="D58" s="155"/>
+      <c r="E58" s="155"/>
+      <c r="F58" s="155"/>
+      <c r="G58" s="155"/>
+      <c r="H58" s="155"/>
+      <c r="I58" s="155"/>
+      <c r="J58" s="155"/>
+    </row>
+    <row r="59" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="155"/>
+      <c r="C59" s="155"/>
+      <c r="D59" s="155"/>
+      <c r="E59" s="155"/>
+      <c r="F59" s="155"/>
+      <c r="G59" s="155"/>
+      <c r="H59" s="155"/>
+      <c r="I59" s="155"/>
+      <c r="J59" s="155"/>
+    </row>
+    <row r="60" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="156" t="str">
         <f>CONCATENATE("2. Que con el pago del dinero anotado en la presente liquidación, queda transada cualquier diferencia relativa al contrato de trabajo extinguido,"," o a cualquier diferencia anterior. Por lo tanto, esta transacción tiene como efecto la terminación de las obligaciones provenientes de la relación laboral que existió entre ",B2," y el trabajador, quienes declaran estar a paz y salvo por todo concepto.")</f>
         <v>2. Que con el pago del dinero anotado en la presente liquidación, queda transada cualquier diferencia relativa al contrato de trabajo extinguido, o a cualquier diferencia anterior. Por lo tanto, esta transacción tiene como efecto la terminación de las obligaciones provenientes de la relación laboral que existió entre A. B. C. LTDA y el trabajador, quienes declaran estar a paz y salvo por todo concepto.</v>
       </c>
-      <c r="C60" s="144"/>
-      <c r="D60" s="144"/>
-      <c r="E60" s="144"/>
-      <c r="F60" s="144"/>
-      <c r="G60" s="144"/>
-      <c r="H60" s="144"/>
-      <c r="I60" s="144"/>
-      <c r="J60" s="144"/>
+      <c r="C60" s="156"/>
+      <c r="D60" s="156"/>
+      <c r="E60" s="156"/>
+      <c r="F60" s="156"/>
+      <c r="G60" s="156"/>
+      <c r="H60" s="156"/>
+      <c r="I60" s="156"/>
+      <c r="J60" s="156"/>
       <c r="K60" s="119"/>
     </row>
-    <row r="61" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="144"/>
-      <c r="C61" s="144"/>
-      <c r="D61" s="144"/>
-      <c r="E61" s="144"/>
-      <c r="F61" s="144"/>
-      <c r="G61" s="144"/>
-      <c r="H61" s="144"/>
-      <c r="I61" s="144"/>
-      <c r="J61" s="144"/>
-    </row>
-    <row r="62" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="144"/>
-      <c r="C62" s="144"/>
-      <c r="D62" s="144"/>
-      <c r="E62" s="144"/>
-      <c r="F62" s="144"/>
-      <c r="G62" s="144"/>
-      <c r="H62" s="144"/>
-      <c r="I62" s="144"/>
-      <c r="J62" s="144"/>
-    </row>
-    <row r="63" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="144"/>
-      <c r="C63" s="144"/>
-      <c r="D63" s="144"/>
-      <c r="E63" s="144"/>
-      <c r="F63" s="144"/>
-      <c r="G63" s="144"/>
-      <c r="H63" s="144"/>
-      <c r="I63" s="144"/>
-      <c r="J63" s="144"/>
-    </row>
-    <row r="64" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="142"/>
-      <c r="C64" s="142"/>
-      <c r="D64" s="142"/>
-      <c r="E64" s="142"/>
-      <c r="F64" s="142"/>
-      <c r="G64" s="142"/>
-      <c r="H64" s="142"/>
-      <c r="I64" s="142"/>
-      <c r="J64" s="142"/>
-    </row>
-    <row r="65" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="156"/>
+      <c r="C61" s="156"/>
+      <c r="D61" s="156"/>
+      <c r="E61" s="156"/>
+      <c r="F61" s="156"/>
+      <c r="G61" s="156"/>
+      <c r="H61" s="156"/>
+      <c r="I61" s="156"/>
+      <c r="J61" s="156"/>
+    </row>
+    <row r="62" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="156"/>
+      <c r="C62" s="156"/>
+      <c r="D62" s="156"/>
+      <c r="E62" s="156"/>
+      <c r="F62" s="156"/>
+      <c r="G62" s="156"/>
+      <c r="H62" s="156"/>
+      <c r="I62" s="156"/>
+      <c r="J62" s="156"/>
+    </row>
+    <row r="63" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="156"/>
+      <c r="C63" s="156"/>
+      <c r="D63" s="156"/>
+      <c r="E63" s="156"/>
+      <c r="F63" s="156"/>
+      <c r="G63" s="156"/>
+      <c r="H63" s="156"/>
+      <c r="I63" s="156"/>
+      <c r="J63" s="156"/>
+    </row>
+    <row r="64" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="154"/>
+      <c r="C64" s="154"/>
+      <c r="D64" s="154"/>
+      <c r="E64" s="154"/>
+      <c r="F64" s="154"/>
+      <c r="G64" s="154"/>
+      <c r="H64" s="154"/>
+      <c r="I64" s="154"/>
+      <c r="J64" s="154"/>
+    </row>
+    <row r="65" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -2911,7 +2911,7 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="79"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -2922,7 +2922,7 @@
       <c r="I66" s="23"/>
       <c r="J66" s="79"/>
     </row>
-    <row r="67" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="24" t="str">
         <f>C7</f>
         <v>PEPITO PEREZ</v>
@@ -2937,7 +2937,7 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="24" t="str">
         <f>CONCATENATE(B8,C8)</f>
         <v>C.C.: XX.XXX.XXX</v>
@@ -2952,7 +2952,7 @@
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -2964,7 +2964,7 @@
       <c r="I69" s="24"/>
       <c r="J69" s="3"/>
     </row>
-    <row r="70" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="80" t="s">
         <v>81</v>
       </c>
@@ -2977,7 +2977,7 @@
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
     </row>
-    <row r="71" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="80" t="s">
         <v>82</v>
       </c>
@@ -2990,7 +2990,7 @@
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="15"/>
@@ -3001,7 +3001,7 @@
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
     </row>
-    <row r="73" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="118"/>
       <c r="D73" s="120"/>
       <c r="E73" s="121"/>
@@ -3011,7 +3011,7 @@
       <c r="I73" s="124"/>
       <c r="J73" s="125"/>
     </row>
-    <row r="74" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="115"/>
       <c r="C74" s="126"/>
       <c r="D74" s="120"/>
@@ -3022,7 +3022,7 @@
       <c r="I74" s="124"/>
       <c r="J74" s="125"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B75" s="115"/>
       <c r="C75" s="125"/>
       <c r="D75" s="120"/>
@@ -3033,7 +3033,7 @@
       <c r="I75" s="124"/>
       <c r="J75" s="125"/>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B76" s="115"/>
       <c r="C76" s="121"/>
       <c r="E76" s="120"/>
@@ -3043,7 +3043,7 @@
       <c r="I76" s="124"/>
       <c r="J76" s="125"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B77" s="115"/>
       <c r="C77" s="128"/>
       <c r="E77" s="120"/>
@@ -3053,7 +3053,7 @@
       <c r="I77" s="129"/>
       <c r="J77" s="125"/>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B78" s="115"/>
       <c r="C78" s="130"/>
       <c r="D78" s="120"/>
@@ -3063,7 +3063,7 @@
       <c r="H78" s="123"/>
       <c r="I78" s="124"/>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B79" s="115"/>
       <c r="C79" s="131"/>
       <c r="D79" s="120"/>
@@ -3074,7 +3074,7 @@
       <c r="I79" s="132"/>
       <c r="J79" s="125"/>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D80" s="120"/>
       <c r="E80" s="120"/>
       <c r="F80" s="120"/>
@@ -3083,7 +3083,7 @@
       <c r="I80" s="133"/>
       <c r="J80" s="125"/>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B81" s="115"/>
       <c r="D81" s="120"/>
       <c r="E81" s="120"/>
@@ -3093,7 +3093,7 @@
       <c r="I81" s="124"/>
       <c r="J81" s="125"/>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B82" s="115"/>
       <c r="C82" s="135"/>
       <c r="F82" s="123"/>
@@ -3102,7 +3102,7 @@
       <c r="I82" s="124"/>
       <c r="J82" s="125"/>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B83" s="115"/>
       <c r="C83" s="135"/>
       <c r="F83" s="123"/>
@@ -3111,7 +3111,7 @@
       <c r="I83" s="124"/>
       <c r="J83" s="125"/>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B84" s="115"/>
       <c r="C84" s="128"/>
       <c r="F84" s="123"/>
@@ -3120,20 +3120,37 @@
       <c r="I84" s="129"/>
       <c r="J84" s="125"/>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B85" s="115"/>
       <c r="C85" s="128"/>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B86" s="115"/>
       <c r="C86" s="128"/>
     </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B87" s="115"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="33">
+    <mergeCell ref="B64:J64"/>
+    <mergeCell ref="B57:J59"/>
+    <mergeCell ref="B60:J63"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C53:J54"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B49:I49"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="B44:J44"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B4:J4"/>
@@ -3150,23 +3167,6 @@
     <mergeCell ref="E27:I27"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="C7:G7"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="B44:J44"/>
-    <mergeCell ref="B64:J64"/>
-    <mergeCell ref="B57:J59"/>
-    <mergeCell ref="B60:J63"/>
-    <mergeCell ref="B32:J32"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C53:J54"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B49:I49"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3189,23 +3189,23 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="88" customWidth="1"/>
-    <col min="2" max="6" width="11.44140625" style="88"/>
-    <col min="7" max="7" width="23.5546875" style="88" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="88"/>
+    <col min="1" max="1" width="6.85546875" style="88" customWidth="1"/>
+    <col min="2" max="6" width="11.42578125" style="88"/>
+    <col min="7" max="7" width="23.5703125" style="88" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="165" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="166"/>
       <c r="D2" s="167"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="89" t="s">
         <v>41</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="92">
         <v>2020</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>70500</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="95">
         <v>2019</v>
       </c>
@@ -3238,8 +3238,8 @@
         <v>72000</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="165" t="s">
         <v>86</v>
       </c>
@@ -3253,7 +3253,7 @@
       <c r="I8" s="166"/>
       <c r="J8" s="167"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="62" t="s">
         <v>32</v>
       </c>
@@ -3271,17 +3271,17 @@
       </c>
       <c r="H9" s="98">
         <f>Liquidación!J14</f>
-        <v>1350000</v>
+        <v>2500000</v>
       </c>
       <c r="I9" s="88" t="s">
         <v>91</v>
       </c>
       <c r="J9" s="99">
         <f>H9/240</f>
-        <v>5625</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+        <v>10416.666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="64" t="s">
         <v>20</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="64" t="s">
         <v>21</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="64" t="s">
         <v>22</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="64" t="s">
         <v>23</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="64" t="s">
         <v>24</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="64" t="s">
         <v>25</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="64" t="s">
         <v>26</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="64" t="s">
         <v>27</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="64" t="s">
         <v>28</v>
       </c>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="J18" s="98"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="64" t="s">
         <v>29</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="64" t="s">
         <v>30</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="64" t="s">
         <v>31</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="65" t="s">
         <v>85</v>
       </c>
@@ -3594,22 +3594,22 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="88" customWidth="1"/>
-    <col min="2" max="11" width="12.6640625" style="88" customWidth="1"/>
-    <col min="12" max="16384" width="11.44140625" style="88"/>
+    <col min="1" max="1" width="22.7109375" style="88" customWidth="1"/>
+    <col min="2" max="11" width="12.7109375" style="88" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="140">
         <f>ROUND(Liquidación!J51,0)</f>
-        <v>1114355</v>
+        <v>1342576</v>
       </c>
       <c r="B2" s="168" t="str">
         <f>CONCATENATE(B22,C22,D22,E22,F22,G22,H22,I22,J22,K22,A3)</f>
-        <v>UN MILLÓN CIENTO CATORCE MIL TRESCIENTOS CINCUENTA Y CINCO PESOS M/C</v>
+        <v>UN MILLÓN TRESCIENTOS CUARENTA Y DOS MIL QUINIENTOS SETENTA Y SEIS PESOS M/C</v>
       </c>
       <c r="C2" s="169"/>
       <c r="D2" s="169"/>
@@ -3621,52 +3621,52 @@
       <c r="J2" s="169"/>
       <c r="K2" s="170"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="88" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="92" t="str">
         <f>RIGHT($A$2,(10))</f>
-        <v>1114355</v>
+        <v>1342576</v>
       </c>
       <c r="C3" s="88" t="str">
         <f>RIGHT($A$2,(9))</f>
-        <v>1114355</v>
+        <v>1342576</v>
       </c>
       <c r="D3" s="88" t="str">
         <f>RIGHT($A$2,(8))</f>
-        <v>1114355</v>
+        <v>1342576</v>
       </c>
       <c r="E3" s="88" t="str">
         <f>RIGHT($A$2,(7))</f>
-        <v>1114355</v>
+        <v>1342576</v>
       </c>
       <c r="F3" s="88" t="str">
         <f>RIGHT($A$2,(6))</f>
-        <v>114355</v>
+        <v>342576</v>
       </c>
       <c r="G3" s="88" t="str">
         <f>RIGHT($A$2,(5))</f>
-        <v>14355</v>
+        <v>42576</v>
       </c>
       <c r="H3" s="88" t="str">
         <f>RIGHT($A$2,(4))</f>
-        <v>4355</v>
+        <v>2576</v>
       </c>
       <c r="I3" s="88" t="str">
         <f>RIGHT($A$2,(3))</f>
-        <v>355</v>
+        <v>576</v>
       </c>
       <c r="J3" s="88" t="str">
         <f>RIGHT($A$2,(2))</f>
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="K3" s="105" t="str">
         <f>RIGHT($A$2)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="106"/>
       <c r="B4" s="92">
         <f t="shared" ref="B4:J4" si="0">LEN(B3)</f>
@@ -3709,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="107"/>
       <c r="B5" s="92" t="b">
         <f>IF(B4=10,TRUE,FALSE)</f>
@@ -3752,7 +3752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="107"/>
       <c r="B6" s="92" t="str">
         <f t="shared" ref="B6:K6" si="1">MID(B3,1,1)</f>
@@ -3772,30 +3772,30 @@
       </c>
       <c r="F6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K6" s="105" t="str">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="107"/>
       <c r="B7" s="92">
         <f t="shared" ref="B7:G7" si="2">IF(B5=TRUE,(VALUE(B6)),0)</f>
@@ -3815,35 +3815,35 @@
       </c>
       <c r="F7" s="88">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" s="88">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H7" s="88">
         <f>IF(H5=TRUE,(VALUE(H6)),)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" s="88">
         <f>IF(I5=TRUE,(VALUE(I6)),0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J7" s="88">
         <f>IF(J5=TRUE,(VALUE(J6)),0)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K7" s="105">
         <f>IF(K5=TRUE,(VALUE(K6)),0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="107"/>
       <c r="B8" s="92"/>
       <c r="K8" s="105"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="107"/>
       <c r="B9" s="108">
         <f t="shared" ref="B9:K9" si="3">B7</f>
@@ -3863,46 +3863,46 @@
       </c>
       <c r="F9" s="109">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="109">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H9" s="109">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I9" s="109">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J9" s="109">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K9" s="110">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L9" s="109"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="107"/>
       <c r="B10" s="92"/>
       <c r="K10" s="105"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="107"/>
       <c r="B11" s="92"/>
       <c r="K11" s="105"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="107"/>
       <c r="B12" s="92"/>
       <c r="K12" s="105"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="107"/>
       <c r="B13" s="92" t="b">
         <f>IF(B9=1," MIL",IF(B9=2," DOS MIL",IF(B9=3," TRES MIL",IF(B9=4," CUATRO MIL",IF(B9=5," CINCO MIL")))))</f>
@@ -3922,30 +3922,30 @@
       </c>
       <c r="F13" s="88" t="str">
         <f>IF(F9=1," CIENTO",IF(F9=2," DOSCIENTOS",IF(F9=3," TRESCIENTOS",IF(F9=4," CUATROCIENTOS",IF(F9=5," QUINIENTOS")))))</f>
-        <v xml:space="preserve"> CIENTO</v>
+        <v xml:space="preserve"> TRESCIENTOS</v>
       </c>
       <c r="G13" s="88" t="str">
         <f>IF(G9=1," DIEZ Y",IF(G9=2," VEINTI",IF(G9=3," TREINTA Y",IF(G9=4," CUARENTA Y",IF(G9=5," CINCUENTA Y")))))</f>
-        <v xml:space="preserve"> DIEZ Y</v>
+        <v xml:space="preserve"> CUARENTA Y</v>
       </c>
       <c r="H13" s="88" t="str">
         <f>IF(H9=1," UN MIL",IF(H9=2," DOS MIL",IF(H9=3," TRES MIL",IF(H9=4," CUATRO MIL",IF(H9=5," CINCO MIL")))))</f>
-        <v xml:space="preserve"> CUATRO MIL</v>
+        <v xml:space="preserve"> DOS MIL</v>
       </c>
       <c r="I13" s="88" t="str">
         <f>IF(I9=1," CIENTO",IF(I9=2," DOSCIENTOS",IF(I9=3," TRESCIENTOS",IF(I9=4," CUATROCIENTOS",IF(I9=5," QUINIENTOS")))))</f>
-        <v xml:space="preserve"> TRESCIENTOS</v>
-      </c>
-      <c r="J13" s="88" t="str">
+        <v xml:space="preserve"> QUINIENTOS</v>
+      </c>
+      <c r="J13" s="88" t="b">
         <f>IF(J9=1," DIEZ Y",IF(J9=2," VEINTI",IF(J9=3," TREINTA Y",IF(J9=4," CUARENTA Y",IF(J9=5," CINCUENTA Y")))))</f>
-        <v xml:space="preserve"> CINCUENTA Y</v>
-      </c>
-      <c r="K13" s="105" t="str">
+        <v>0</v>
+      </c>
+      <c r="K13" s="105" t="b">
         <f>IF(K9=1," UN",IF(K9=2," DOS",IF(K9=3," TRES",IF(K9=4," CUATRO",IF(K9=5," CINCO")))))</f>
-        <v xml:space="preserve"> CINCO</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="107"/>
       <c r="B14" s="92" t="b">
         <f>IF(B9=6," SEIS MIL",IF(B9=7," SIETE MIL",IF(B9=8," OCHO MIL",IF(B9=9," NUEVE MIL"))))</f>
@@ -3979,16 +3979,16 @@
         <f>IF(I9=6," SEISCIENTOS",IF(I9=7," SETECIENTOS",IF(I9=8," OCHOCIENTOS",IF(I9=9," NOVECIENTOS"))))</f>
         <v>0</v>
       </c>
-      <c r="J14" s="88" t="b">
+      <c r="J14" s="88" t="str">
         <f>IF(J9=6," SESENTA Y",IF(J9=7," SETENTA Y",IF(J9=8," OCHENTA Y",IF(J9=9," NOVENTA Y"))))</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="105" t="b">
+        <v xml:space="preserve"> SETENTA Y</v>
+      </c>
+      <c r="K14" s="105" t="str">
         <f>IF(K9=6," SEIS",IF(K9=7," SIETE",IF(K9=8," OCHO",IF(K9=9," NUEVE"))))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> SEIS</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="107"/>
       <c r="B15" s="92" t="b">
         <f t="shared" ref="B15:K15" si="4">IF(B13=FALSE,B14,B13)</f>
@@ -4008,30 +4008,30 @@
       </c>
       <c r="F15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> CIENTO</v>
+        <v xml:space="preserve"> TRESCIENTOS</v>
       </c>
       <c r="G15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> DIEZ Y</v>
+        <v xml:space="preserve"> CUARENTA Y</v>
       </c>
       <c r="H15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> CUATRO MIL</v>
+        <v xml:space="preserve"> DOS MIL</v>
       </c>
       <c r="I15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> TRESCIENTOS</v>
+        <v xml:space="preserve"> QUINIENTOS</v>
       </c>
       <c r="J15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> CINCUENTA Y</v>
+        <v xml:space="preserve"> SETENTA Y</v>
       </c>
       <c r="K15" s="105" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> CINCO</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> SEIS</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="107"/>
       <c r="B16" s="92" t="str">
         <f>CONCATENATE(A9,B9,C9,D9,E9,)</f>
@@ -4051,30 +4051,30 @@
       </c>
       <c r="F16" s="88" t="str">
         <f>CONCATENATE(F9,G9,H9)</f>
-        <v>114</v>
+        <v>342</v>
       </c>
       <c r="G16" s="88" t="str">
         <f>CONCATENATE(G9,H9)</f>
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="H16" s="88" t="str">
         <f>CONCATENATE(G9,H9)</f>
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I16" s="88" t="str">
         <f>CONCATENATE(I9,J9,K9)</f>
-        <v>355</v>
+        <v>576</v>
       </c>
       <c r="J16" s="88" t="str">
         <f>CONCATENATE(J9,K9)</f>
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="K16" s="105" t="str">
         <f>CONCATENATE(J9,K9)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="107"/>
       <c r="B17" s="92" t="str">
         <f>IF(B9=0,"",IF(B16="00000","",IF(B16="10000","",IF(B16="11000","",IF(B16="12000","",IF(B16="13000","",IF(B16="14000","",IF(B16="15000",""))))))))</f>
@@ -4096,13 +4096,13 @@
         <f>IF(F9=0,"",IF(F16="000","",IF(F16="100"," CIEN MIL" )))</f>
         <v>0</v>
       </c>
-      <c r="G17" s="88" t="str">
+      <c r="G17" s="88" t="b">
         <f>IF(G9=0,"",IF(G16="00","",IF(G16="10"," DIEZ MIL",IF(G16="11"," ONCE MIL",IF(G16="12"," DOCE MIL",IF(G16="13"," TRECE MIL",IF(G16="14"," CATORCE MIL",IF(G16="15"," QUINCE MIL"))))))))</f>
-        <v xml:space="preserve"> CATORCE MIL</v>
-      </c>
-      <c r="H17" s="88" t="str">
+        <v>0</v>
+      </c>
+      <c r="H17" s="88" t="b">
         <f>IF(H9=0,"",IF(H16="00","",IF(H16="10","",IF(H16="11","",IF(H16="12","",IF(H16="13","",IF(H16="14","",IF(H16="15",""))))))))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I17" s="88" t="b">
         <f>IF(I9=0,"",IF(I16="000","",IF(I16="100"," CIEN" )))</f>
@@ -4117,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="107"/>
       <c r="B18" s="92" t="str">
         <f>IF(B17=FALSE,B15,B17)</f>
@@ -4145,11 +4145,11 @@
       </c>
       <c r="H18" s="88" t="str">
         <f>IF(H17=FALSE,H15,H17)</f>
-        <v/>
+        <v xml:space="preserve"> DOS MIL</v>
       </c>
       <c r="I18" s="88" t="str">
         <f>IF(I17=FALSE,I15,I17)</f>
-        <v xml:space="preserve"> TRESCIENTOS</v>
+        <v xml:space="preserve"> QUINIENTOS</v>
       </c>
       <c r="J18" s="88" t="b">
         <f>IF(J16="20"," VEINTE",IF(J16="30"," TREINTA",IF(J16="40"," CUARENTA",IF(J16="50"," CINCUENTA",IF(J16="60"," SESENTA",IF(J16="80"," OCHENTA",IF(J16="90"," NOVENTA")))))))</f>
@@ -4157,10 +4157,10 @@
       </c>
       <c r="K18" s="105" t="str">
         <f>IF(K17=FALSE,K15,K17)</f>
-        <v xml:space="preserve"> CINCO</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> SEIS</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="107"/>
       <c r="B19" s="92"/>
       <c r="C19" s="88" t="str">
@@ -4177,19 +4177,19 @@
       </c>
       <c r="F19" s="88" t="str">
         <f>IF(F17=FALSE,F15,F17)</f>
-        <v xml:space="preserve"> CIENTO</v>
+        <v xml:space="preserve"> TRESCIENTOS</v>
       </c>
       <c r="G19" s="88" t="str">
         <f>IF(G17=FALSE,G15,G17)</f>
-        <v xml:space="preserve"> CATORCE MIL</v>
+        <v xml:space="preserve"> CUARENTA Y</v>
       </c>
       <c r="J19" s="88" t="str">
         <f>IF(J17=FALSE,J15,J17)</f>
-        <v xml:space="preserve"> CINCUENTA Y</v>
+        <v xml:space="preserve"> SETENTA Y</v>
       </c>
       <c r="K19" s="105"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="107"/>
       <c r="B20" s="92"/>
       <c r="C20" s="88" t="str">
@@ -4206,24 +4206,24 @@
       </c>
       <c r="F20" s="88" t="str">
         <f>IF(F18=FALSE,F19,F18)</f>
-        <v xml:space="preserve"> CIENTO</v>
+        <v xml:space="preserve"> TRESCIENTOS</v>
       </c>
       <c r="G20" s="88" t="str">
         <f>IF(G18=FALSE,G19,G18)</f>
-        <v xml:space="preserve"> CATORCE MIL</v>
+        <v xml:space="preserve"> CUARENTA Y</v>
       </c>
       <c r="J20" s="88" t="str">
         <f>IF(J18=FALSE,J19,J18)</f>
-        <v xml:space="preserve"> CINCUENTA Y</v>
+        <v xml:space="preserve"> SETENTA Y</v>
       </c>
       <c r="K20" s="105"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="107"/>
       <c r="B21" s="92"/>
       <c r="K21" s="105"/>
     </row>
-    <row r="22" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="107"/>
       <c r="B22" s="95" t="str">
         <f>B18</f>
@@ -4243,30 +4243,30 @@
       </c>
       <c r="F22" s="111" t="str">
         <f>F20</f>
-        <v xml:space="preserve"> CIENTO</v>
+        <v xml:space="preserve"> TRESCIENTOS</v>
       </c>
       <c r="G22" s="111" t="str">
         <f>G20</f>
-        <v xml:space="preserve"> CATORCE MIL</v>
+        <v xml:space="preserve"> CUARENTA Y</v>
       </c>
       <c r="H22" s="111" t="str">
         <f>H18</f>
-        <v/>
+        <v xml:space="preserve"> DOS MIL</v>
       </c>
       <c r="I22" s="111" t="str">
         <f>I18</f>
-        <v xml:space="preserve"> TRESCIENTOS</v>
+        <v xml:space="preserve"> QUINIENTOS</v>
       </c>
       <c r="J22" s="111" t="str">
         <f>J20</f>
-        <v xml:space="preserve"> CINCUENTA Y</v>
+        <v xml:space="preserve"> SETENTA Y</v>
       </c>
       <c r="K22" s="112" t="str">
         <f>K18</f>
-        <v xml:space="preserve"> CINCO</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v xml:space="preserve"> SEIS</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I25" s="141"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se finaliza todo el proceso de calculos y elaboracion completa del PDF y se daria por terminada la aplicacion a nivel de codigo fuente. Queda pendiente elaborar el archivo .exe y realizar pruebas en distintos computadores.
</commit_message>
<xml_diff>
--- a/Base para desarrollo de liquidacion empleados.xlsx
+++ b/Base para desarrollo de liquidacion empleados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Documents\Python\004. Liquidacion de empleados\Liquidacion_de_empleados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5175D121-F71C-4CFF-90C8-6F3B2A414B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C87A289-5165-491B-919A-9E2A362D0408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1419,6 +1419,66 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="34" fillId="25" borderId="10" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="34" fillId="25" borderId="11" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="34" fillId="25" borderId="12" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="29" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="29" fillId="0" borderId="14" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="29" fillId="0" borderId="17" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="29" fillId="0" borderId="18" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="24" fillId="0" borderId="15" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="24" fillId="0" borderId="17" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="15" fontId="27" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1430,68 +1490,8 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="15" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="17" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="34" fillId="25" borderId="10" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="34" fillId="25" borderId="12" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="168" fontId="25" fillId="0" borderId="13" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="34" fillId="25" borderId="11" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="29" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="29" fillId="0" borderId="14" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="29" fillId="0" borderId="17" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="29" fillId="0" borderId="18" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1843,8 +1843,8 @@
   </sheetPr>
   <dimension ref="B1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1866,43 +1866,43 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="142" t="s">
+      <c r="B2" s="161" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="161"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="161"/>
+      <c r="I2" s="161"/>
+      <c r="J2" s="161"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="161" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
-      <c r="H3" s="142"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="142"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="162" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="143"/>
-      <c r="J4" s="143"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="162"/>
+      <c r="G4" s="162"/>
+      <c r="H4" s="162"/>
+      <c r="I4" s="162"/>
+      <c r="J4" s="162"/>
       <c r="K4" s="114"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1934,13 +1934,13 @@
       <c r="B7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="C7" s="160" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="152"/>
-      <c r="E7" s="152"/>
-      <c r="F7" s="152"/>
-      <c r="G7" s="152"/>
+      <c r="D7" s="160"/>
+      <c r="E7" s="160"/>
+      <c r="F7" s="160"/>
+      <c r="G7" s="160"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -1949,11 +1949,11 @@
       <c r="B8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="144" t="s">
+      <c r="C8" s="163" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="144"/>
-      <c r="E8" s="144"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1964,11 +1964,11 @@
       <c r="B9" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="153" t="s">
+      <c r="C9" s="159" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="153"/>
-      <c r="E9" s="153"/>
+      <c r="D9" s="159"/>
+      <c r="E9" s="159"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1979,11 +1979,11 @@
       <c r="B10" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="152" t="s">
+      <c r="C10" s="160" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="152"/>
-      <c r="E10" s="152"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="160"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2013,19 +2013,19 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="147" t="s">
+      <c r="B13" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="148"/>
+      <c r="C13" s="147"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="147" t="s">
+      <c r="E13" s="145" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="151"/>
-      <c r="G13" s="151"/>
-      <c r="H13" s="151"/>
-      <c r="I13" s="151"/>
-      <c r="J13" s="148"/>
+      <c r="F13" s="146"/>
+      <c r="G13" s="146"/>
+      <c r="H13" s="146"/>
+      <c r="I13" s="146"/>
+      <c r="J13" s="147"/>
     </row>
     <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="75" t="s">
@@ -2088,8 +2088,7 @@
         <v>83</v>
       </c>
       <c r="C17" s="30">
-        <f>Datos!J17</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="31" t="s">
@@ -2109,7 +2108,7 @@
         <v>63</v>
       </c>
       <c r="C18" s="78">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="36" t="s">
@@ -2120,7 +2119,7 @@
       <c r="H18" s="38"/>
       <c r="I18" s="34"/>
       <c r="J18" s="72">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2135,35 +2134,35 @@
       <c r="J19" s="85"/>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="147" t="s">
+      <c r="B20" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="148"/>
+      <c r="C20" s="147"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="147" t="s">
+      <c r="E20" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="151"/>
-      <c r="G20" s="151"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="151"/>
-      <c r="J20" s="148"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="146"/>
+      <c r="I20" s="146"/>
+      <c r="J20" s="147"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="75" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="67">
-        <v>44932</v>
+        <v>45194</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="149" t="s">
+      <c r="E21" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="150"/>
-      <c r="G21" s="150"/>
-      <c r="H21" s="150"/>
-      <c r="I21" s="150"/>
+      <c r="F21" s="158"/>
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="158"/>
       <c r="J21" s="67">
         <v>44129</v>
       </c>
@@ -2173,16 +2172,16 @@
         <v>7</v>
       </c>
       <c r="C22" s="67">
-        <v>44927</v>
+        <v>45108</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="149" t="s">
+      <c r="E22" s="164" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
-      <c r="H22" s="150"/>
-      <c r="I22" s="150"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="158"/>
       <c r="J22" s="67">
         <v>44108</v>
       </c>
@@ -2193,16 +2192,16 @@
       </c>
       <c r="C23" s="43">
         <f>DAYS360(C22,C21)+1</f>
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="145" t="s">
+      <c r="E23" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="146"/>
-      <c r="G23" s="146"/>
-      <c r="H23" s="146"/>
-      <c r="I23" s="146"/>
+      <c r="F23" s="157"/>
+      <c r="G23" s="157"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="157"/>
       <c r="J23" s="43">
         <f>DAYS360(J22,J21)+1</f>
         <v>22</v>
@@ -2220,19 +2219,19 @@
       <c r="J24" s="84"/>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="147" t="s">
+      <c r="B25" s="145" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="148"/>
+      <c r="C25" s="147"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="147" t="s">
+      <c r="E25" s="145" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="151"/>
-      <c r="G25" s="151"/>
-      <c r="H25" s="151"/>
-      <c r="I25" s="151"/>
-      <c r="J25" s="148"/>
+      <c r="F25" s="146"/>
+      <c r="G25" s="146"/>
+      <c r="H25" s="146"/>
+      <c r="I25" s="146"/>
+      <c r="J25" s="147"/>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="75" t="s">
@@ -2242,13 +2241,13 @@
         <v>44933</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="149" t="s">
+      <c r="E26" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="150"/>
-      <c r="G26" s="150"/>
-      <c r="H26" s="150"/>
-      <c r="I26" s="150"/>
+      <c r="F26" s="158"/>
+      <c r="G26" s="158"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="158"/>
       <c r="J26" s="67">
         <v>44129</v>
       </c>
@@ -2261,13 +2260,13 @@
         <v>39980</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="149" t="s">
+      <c r="E27" s="164" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="150"/>
-      <c r="G27" s="150"/>
-      <c r="H27" s="150"/>
-      <c r="I27" s="150"/>
+      <c r="F27" s="158"/>
+      <c r="G27" s="158"/>
+      <c r="H27" s="158"/>
+      <c r="I27" s="158"/>
       <c r="J27" s="67">
         <v>44108</v>
       </c>
@@ -2281,13 +2280,13 @@
         <v>203.41666666666666</v>
       </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="145" t="s">
+      <c r="E28" s="156" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
-      <c r="H28" s="146"/>
-      <c r="I28" s="146"/>
+      <c r="F28" s="157"/>
+      <c r="G28" s="157"/>
+      <c r="H28" s="157"/>
+      <c r="I28" s="157"/>
       <c r="J28" s="43">
         <f>DAYS360(J27,J26)+1</f>
         <v>22</v>
@@ -2317,11 +2316,11 @@
         <v>8.4166666666666572</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="150"/>
-      <c r="H30" s="150"/>
-      <c r="I30" s="150"/>
+      <c r="E30" s="158"/>
+      <c r="F30" s="158"/>
+      <c r="G30" s="158"/>
+      <c r="H30" s="158"/>
+      <c r="I30" s="158"/>
       <c r="J30" s="16"/>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2336,31 +2335,31 @@
       <c r="J31" s="84"/>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="147" t="s">
+      <c r="B32" s="145" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="151"/>
-      <c r="D32" s="151"/>
-      <c r="E32" s="151"/>
-      <c r="F32" s="151"/>
-      <c r="G32" s="151"/>
-      <c r="H32" s="151"/>
-      <c r="I32" s="151"/>
-      <c r="J32" s="148"/>
+      <c r="C32" s="146"/>
+      <c r="D32" s="146"/>
+      <c r="E32" s="146"/>
+      <c r="F32" s="146"/>
+      <c r="G32" s="146"/>
+      <c r="H32" s="146"/>
+      <c r="I32" s="146"/>
+      <c r="J32" s="147"/>
     </row>
     <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="164" t="s">
+      <c r="C33" s="155" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="164"/>
-      <c r="E33" s="164"/>
-      <c r="F33" s="164"/>
-      <c r="G33" s="164"/>
-      <c r="H33" s="164"/>
-      <c r="I33" s="164"/>
+      <c r="D33" s="155"/>
+      <c r="E33" s="155"/>
+      <c r="F33" s="155"/>
+      <c r="G33" s="155"/>
+      <c r="H33" s="155"/>
+      <c r="I33" s="155"/>
       <c r="J33" s="26" t="s">
         <v>77</v>
       </c>
@@ -2412,7 +2411,7 @@
       </c>
       <c r="G35" s="10">
         <f>J23-$J$18</f>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>9</v>
@@ -2420,7 +2419,7 @@
       <c r="I35" s="18"/>
       <c r="J35" s="17">
         <f t="shared" ref="J35:J41" si="0">((C35/E35)*G35)</f>
-        <v>161944.44444444444</v>
+        <v>139861.11111111112</v>
       </c>
     </row>
     <row r="36" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2429,7 +2428,7 @@
       </c>
       <c r="C36" s="19">
         <f>$J$35</f>
-        <v>161944.44444444444</v>
+        <v>139861.11111111112</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>8</v>
@@ -2442,7 +2441,7 @@
       </c>
       <c r="G36" s="10">
         <f>J28-$J$18</f>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H36" s="19" t="s">
         <v>10</v>
@@ -2452,7 +2451,7 @@
       </c>
       <c r="J36" s="17">
         <f>(((C36/E36)*G36)*I36)</f>
-        <v>1187.5925925925926</v>
+        <v>885.78703703703707</v>
       </c>
     </row>
     <row r="37" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2474,7 +2473,7 @@
       </c>
       <c r="G37" s="10">
         <f>C23</f>
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>9</v>
@@ -2482,7 +2481,7 @@
       <c r="I37" s="18"/>
       <c r="J37" s="17">
         <f t="shared" si="0"/>
-        <v>44166.666666666672</v>
+        <v>625694.4444444445</v>
       </c>
     </row>
     <row r="38" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,13 +2503,13 @@
       </c>
       <c r="G38" s="3">
         <f>C18</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="18"/>
       <c r="J38" s="17">
         <f t="shared" si="0"/>
-        <v>500000</v>
+        <v>666666.66666666663</v>
       </c>
       <c r="M38" s="117"/>
     </row>
@@ -2527,7 +2526,7 @@
       <c r="I39" s="18"/>
       <c r="J39" s="17">
         <f>C17</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2567,29 +2566,29 @@
       </c>
       <c r="G41" s="3">
         <f>C18</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="44">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="42" spans="2:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="145" t="s">
+      <c r="B42" s="156" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="146"/>
-      <c r="D42" s="146"/>
-      <c r="E42" s="146"/>
-      <c r="F42" s="146"/>
-      <c r="G42" s="146"/>
-      <c r="H42" s="146"/>
-      <c r="I42" s="146"/>
+      <c r="C42" s="157"/>
+      <c r="D42" s="157"/>
+      <c r="E42" s="157"/>
+      <c r="F42" s="157"/>
+      <c r="G42" s="157"/>
+      <c r="H42" s="157"/>
+      <c r="I42" s="157"/>
       <c r="J42" s="40">
         <f>SUM(J34:J41)</f>
-        <v>1438687.5925925919</v>
+        <v>2174506.8981481474</v>
       </c>
     </row>
     <row r="43" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2604,17 +2603,17 @@
       <c r="J43" s="87"/>
     </row>
     <row r="44" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="147" t="s">
+      <c r="B44" s="145" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="151"/>
-      <c r="D44" s="151"/>
-      <c r="E44" s="151"/>
-      <c r="F44" s="151"/>
-      <c r="G44" s="151"/>
-      <c r="H44" s="151"/>
-      <c r="I44" s="151"/>
-      <c r="J44" s="148"/>
+      <c r="C44" s="146"/>
+      <c r="D44" s="146"/>
+      <c r="E44" s="146"/>
+      <c r="F44" s="146"/>
+      <c r="G44" s="146"/>
+      <c r="H44" s="146"/>
+      <c r="I44" s="146"/>
+      <c r="J44" s="147"/>
     </row>
     <row r="45" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="50" t="s">
@@ -2624,11 +2623,11 @@
         <v>79</v>
       </c>
       <c r="D45" s="76"/>
-      <c r="E45" s="157" t="s">
+      <c r="E45" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="157"/>
-      <c r="G45" s="157"/>
+      <c r="F45" s="148"/>
+      <c r="G45" s="148"/>
       <c r="H45" s="48"/>
       <c r="I45" s="49"/>
       <c r="J45" s="51" t="s">
@@ -2643,17 +2642,17 @@
         <v>0.04</v>
       </c>
       <c r="D46" s="15"/>
-      <c r="E46" s="158">
+      <c r="E46" s="149">
         <f>IF($J$38&lt;0,$J$34+$J$39,$J$38+$J$39+$J$34)</f>
-        <v>1201388.8888888881</v>
-      </c>
-      <c r="F46" s="158"/>
+        <v>1368065.5555555546</v>
+      </c>
+      <c r="F46" s="149"/>
       <c r="G46" s="21"/>
       <c r="H46" s="19"/>
       <c r="I46" s="21"/>
       <c r="J46" s="52">
         <f>(SUM(E46:G46)*-C46)</f>
-        <v>-48055.555555555526</v>
+        <v>-54722.622222222184</v>
       </c>
     </row>
     <row r="47" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2664,17 +2663,17 @@
         <v>0.04</v>
       </c>
       <c r="D47" s="15"/>
-      <c r="E47" s="158">
+      <c r="E47" s="149">
         <f>IF($J$38&lt;0,$J$34+$J$39,$J$38+$J$39+$J$34)</f>
-        <v>1201388.8888888881</v>
-      </c>
-      <c r="F47" s="158"/>
+        <v>1368065.5555555546</v>
+      </c>
+      <c r="F47" s="149"/>
       <c r="G47" s="45"/>
       <c r="H47" s="19"/>
       <c r="I47" s="21"/>
       <c r="J47" s="52">
         <f>(SUM(E47:G47)*-C47)</f>
-        <v>-48055.555555555526</v>
+        <v>-54722.622222222184</v>
       </c>
     </row>
     <row r="48" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2683,8 +2682,8 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="46"/>
-      <c r="E48" s="163"/>
-      <c r="F48" s="163"/>
+      <c r="E48" s="154"/>
+      <c r="F48" s="154"/>
       <c r="G48" s="21"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -2693,19 +2692,19 @@
       </c>
     </row>
     <row r="49" spans="2:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="145" t="s">
+      <c r="B49" s="156" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="146"/>
-      <c r="D49" s="146"/>
-      <c r="E49" s="146"/>
-      <c r="F49" s="146"/>
-      <c r="G49" s="146"/>
-      <c r="H49" s="146"/>
-      <c r="I49" s="146"/>
+      <c r="C49" s="157"/>
+      <c r="D49" s="157"/>
+      <c r="E49" s="157"/>
+      <c r="F49" s="157"/>
+      <c r="G49" s="157"/>
+      <c r="H49" s="157"/>
+      <c r="I49" s="157"/>
       <c r="J49" s="53">
         <f>SUM(J46:J48)</f>
-        <v>-96111.111111111051</v>
+        <v>-109445.24444444437</v>
       </c>
       <c r="K49" s="118"/>
     </row>
@@ -2734,7 +2733,7 @@
       <c r="I51" s="59"/>
       <c r="J51" s="61">
         <f>+J42+J49</f>
-        <v>1342576.4814814809</v>
+        <v>2065061.6537037031</v>
       </c>
       <c r="K51" s="118"/>
     </row>
@@ -2754,29 +2753,29 @@
       <c r="B53" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="159" t="str">
+      <c r="C53" s="150" t="str">
         <f>'Conversor numeros letras'!B2</f>
-        <v>UN MILLÓN TRESCIENTOS CUARENTA Y DOS MIL QUINIENTOS SETENTA Y SEIS PESOS M/C</v>
-      </c>
-      <c r="D53" s="159"/>
-      <c r="E53" s="159"/>
-      <c r="F53" s="159"/>
-      <c r="G53" s="159"/>
-      <c r="H53" s="159"/>
-      <c r="I53" s="159"/>
-      <c r="J53" s="160"/>
+        <v xml:space="preserve"> DOS MILLONES SESENTA Y CINCO MIL SESENTA Y DOS PESOS M/C</v>
+      </c>
+      <c r="D53" s="150"/>
+      <c r="E53" s="150"/>
+      <c r="F53" s="150"/>
+      <c r="G53" s="150"/>
+      <c r="H53" s="150"/>
+      <c r="I53" s="150"/>
+      <c r="J53" s="151"/>
       <c r="K53" s="118"/>
     </row>
     <row r="54" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="27"/>
-      <c r="C54" s="161"/>
-      <c r="D54" s="161"/>
-      <c r="E54" s="161"/>
-      <c r="F54" s="161"/>
-      <c r="G54" s="161"/>
-      <c r="H54" s="161"/>
-      <c r="I54" s="161"/>
-      <c r="J54" s="162"/>
+      <c r="C54" s="152"/>
+      <c r="D54" s="152"/>
+      <c r="E54" s="152"/>
+      <c r="F54" s="152"/>
+      <c r="G54" s="152"/>
+      <c r="H54" s="152"/>
+      <c r="I54" s="152"/>
+      <c r="J54" s="153"/>
       <c r="K54" s="118"/>
     </row>
     <row r="55" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2806,99 +2805,99 @@
       <c r="K56" s="119"/>
     </row>
     <row r="57" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="155" t="s">
+      <c r="B57" s="143" t="s">
         <v>106</v>
       </c>
-      <c r="C57" s="155"/>
-      <c r="D57" s="155"/>
-      <c r="E57" s="155"/>
-      <c r="F57" s="155"/>
-      <c r="G57" s="155"/>
-      <c r="H57" s="155"/>
-      <c r="I57" s="155"/>
-      <c r="J57" s="155"/>
+      <c r="C57" s="143"/>
+      <c r="D57" s="143"/>
+      <c r="E57" s="143"/>
+      <c r="F57" s="143"/>
+      <c r="G57" s="143"/>
+      <c r="H57" s="143"/>
+      <c r="I57" s="143"/>
+      <c r="J57" s="143"/>
       <c r="K57" s="119"/>
     </row>
     <row r="58" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="155"/>
-      <c r="C58" s="155"/>
-      <c r="D58" s="155"/>
-      <c r="E58" s="155"/>
-      <c r="F58" s="155"/>
-      <c r="G58" s="155"/>
-      <c r="H58" s="155"/>
-      <c r="I58" s="155"/>
-      <c r="J58" s="155"/>
+      <c r="B58" s="143"/>
+      <c r="C58" s="143"/>
+      <c r="D58" s="143"/>
+      <c r="E58" s="143"/>
+      <c r="F58" s="143"/>
+      <c r="G58" s="143"/>
+      <c r="H58" s="143"/>
+      <c r="I58" s="143"/>
+      <c r="J58" s="143"/>
     </row>
     <row r="59" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="155"/>
-      <c r="C59" s="155"/>
-      <c r="D59" s="155"/>
-      <c r="E59" s="155"/>
-      <c r="F59" s="155"/>
-      <c r="G59" s="155"/>
-      <c r="H59" s="155"/>
-      <c r="I59" s="155"/>
-      <c r="J59" s="155"/>
+      <c r="B59" s="143"/>
+      <c r="C59" s="143"/>
+      <c r="D59" s="143"/>
+      <c r="E59" s="143"/>
+      <c r="F59" s="143"/>
+      <c r="G59" s="143"/>
+      <c r="H59" s="143"/>
+      <c r="I59" s="143"/>
+      <c r="J59" s="143"/>
     </row>
     <row r="60" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="156" t="str">
+      <c r="B60" s="144" t="str">
         <f>CONCATENATE("2. Que con el pago del dinero anotado en la presente liquidación, queda transada cualquier diferencia relativa al contrato de trabajo extinguido,"," o a cualquier diferencia anterior. Por lo tanto, esta transacción tiene como efecto la terminación de las obligaciones provenientes de la relación laboral que existió entre ",B2," y el trabajador, quienes declaran estar a paz y salvo por todo concepto.")</f>
         <v>2. Que con el pago del dinero anotado en la presente liquidación, queda transada cualquier diferencia relativa al contrato de trabajo extinguido, o a cualquier diferencia anterior. Por lo tanto, esta transacción tiene como efecto la terminación de las obligaciones provenientes de la relación laboral que existió entre A. B. C. LTDA y el trabajador, quienes declaran estar a paz y salvo por todo concepto.</v>
       </c>
-      <c r="C60" s="156"/>
-      <c r="D60" s="156"/>
-      <c r="E60" s="156"/>
-      <c r="F60" s="156"/>
-      <c r="G60" s="156"/>
-      <c r="H60" s="156"/>
-      <c r="I60" s="156"/>
-      <c r="J60" s="156"/>
+      <c r="C60" s="144"/>
+      <c r="D60" s="144"/>
+      <c r="E60" s="144"/>
+      <c r="F60" s="144"/>
+      <c r="G60" s="144"/>
+      <c r="H60" s="144"/>
+      <c r="I60" s="144"/>
+      <c r="J60" s="144"/>
       <c r="K60" s="119"/>
     </row>
     <row r="61" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="156"/>
-      <c r="C61" s="156"/>
-      <c r="D61" s="156"/>
-      <c r="E61" s="156"/>
-      <c r="F61" s="156"/>
-      <c r="G61" s="156"/>
-      <c r="H61" s="156"/>
-      <c r="I61" s="156"/>
-      <c r="J61" s="156"/>
+      <c r="B61" s="144"/>
+      <c r="C61" s="144"/>
+      <c r="D61" s="144"/>
+      <c r="E61" s="144"/>
+      <c r="F61" s="144"/>
+      <c r="G61" s="144"/>
+      <c r="H61" s="144"/>
+      <c r="I61" s="144"/>
+      <c r="J61" s="144"/>
     </row>
     <row r="62" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="156"/>
-      <c r="C62" s="156"/>
-      <c r="D62" s="156"/>
-      <c r="E62" s="156"/>
-      <c r="F62" s="156"/>
-      <c r="G62" s="156"/>
-      <c r="H62" s="156"/>
-      <c r="I62" s="156"/>
-      <c r="J62" s="156"/>
+      <c r="B62" s="144"/>
+      <c r="C62" s="144"/>
+      <c r="D62" s="144"/>
+      <c r="E62" s="144"/>
+      <c r="F62" s="144"/>
+      <c r="G62" s="144"/>
+      <c r="H62" s="144"/>
+      <c r="I62" s="144"/>
+      <c r="J62" s="144"/>
     </row>
     <row r="63" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="156"/>
-      <c r="C63" s="156"/>
-      <c r="D63" s="156"/>
-      <c r="E63" s="156"/>
-      <c r="F63" s="156"/>
-      <c r="G63" s="156"/>
-      <c r="H63" s="156"/>
-      <c r="I63" s="156"/>
-      <c r="J63" s="156"/>
+      <c r="B63" s="144"/>
+      <c r="C63" s="144"/>
+      <c r="D63" s="144"/>
+      <c r="E63" s="144"/>
+      <c r="F63" s="144"/>
+      <c r="G63" s="144"/>
+      <c r="H63" s="144"/>
+      <c r="I63" s="144"/>
+      <c r="J63" s="144"/>
     </row>
     <row r="64" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="154"/>
-      <c r="C64" s="154"/>
-      <c r="D64" s="154"/>
-      <c r="E64" s="154"/>
-      <c r="F64" s="154"/>
-      <c r="G64" s="154"/>
-      <c r="H64" s="154"/>
-      <c r="I64" s="154"/>
-      <c r="J64" s="154"/>
+      <c r="B64" s="142"/>
+      <c r="C64" s="142"/>
+      <c r="D64" s="142"/>
+      <c r="E64" s="142"/>
+      <c r="F64" s="142"/>
+      <c r="G64" s="142"/>
+      <c r="H64" s="142"/>
+      <c r="I64" s="142"/>
+      <c r="J64" s="142"/>
     </row>
     <row r="65" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
@@ -3134,23 +3133,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="33">
-    <mergeCell ref="B64:J64"/>
-    <mergeCell ref="B57:J59"/>
-    <mergeCell ref="B60:J63"/>
-    <mergeCell ref="B32:J32"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C53:J54"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B49:I49"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="B44:J44"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B4:J4"/>
@@ -3167,6 +3149,23 @@
     <mergeCell ref="E27:I27"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="C7:G7"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="B44:J44"/>
+    <mergeCell ref="B64:J64"/>
+    <mergeCell ref="B57:J59"/>
+    <mergeCell ref="B60:J63"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C53:J54"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B49:I49"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3605,11 +3604,11 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="140">
         <f>ROUND(Liquidación!J51,0)</f>
-        <v>1342576</v>
+        <v>2065062</v>
       </c>
       <c r="B2" s="168" t="str">
         <f>CONCATENATE(B22,C22,D22,E22,F22,G22,H22,I22,J22,K22,A3)</f>
-        <v>UN MILLÓN TRESCIENTOS CUARENTA Y DOS MIL QUINIENTOS SETENTA Y SEIS PESOS M/C</v>
+        <v xml:space="preserve"> DOS MILLONES SESENTA Y CINCO MIL SESENTA Y DOS PESOS M/C</v>
       </c>
       <c r="C2" s="169"/>
       <c r="D2" s="169"/>
@@ -3627,43 +3626,43 @@
       </c>
       <c r="B3" s="92" t="str">
         <f>RIGHT($A$2,(10))</f>
-        <v>1342576</v>
+        <v>2065062</v>
       </c>
       <c r="C3" s="88" t="str">
         <f>RIGHT($A$2,(9))</f>
-        <v>1342576</v>
+        <v>2065062</v>
       </c>
       <c r="D3" s="88" t="str">
         <f>RIGHT($A$2,(8))</f>
-        <v>1342576</v>
+        <v>2065062</v>
       </c>
       <c r="E3" s="88" t="str">
         <f>RIGHT($A$2,(7))</f>
-        <v>1342576</v>
+        <v>2065062</v>
       </c>
       <c r="F3" s="88" t="str">
         <f>RIGHT($A$2,(6))</f>
-        <v>342576</v>
+        <v>065062</v>
       </c>
       <c r="G3" s="88" t="str">
         <f>RIGHT($A$2,(5))</f>
-        <v>42576</v>
+        <v>65062</v>
       </c>
       <c r="H3" s="88" t="str">
         <f>RIGHT($A$2,(4))</f>
-        <v>2576</v>
+        <v>5062</v>
       </c>
       <c r="I3" s="88" t="str">
         <f>RIGHT($A$2,(3))</f>
-        <v>576</v>
+        <v>062</v>
       </c>
       <c r="J3" s="88" t="str">
         <f>RIGHT($A$2,(2))</f>
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="K3" s="105" t="str">
         <f>RIGHT($A$2)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -3756,43 +3755,43 @@
       <c r="A6" s="107"/>
       <c r="B6" s="92" t="str">
         <f t="shared" ref="B6:K6" si="1">MID(B3,1,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J6" s="88" t="str">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K6" s="105" t="str">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -3811,31 +3810,31 @@
       </c>
       <c r="E7" s="88">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="88">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G7" s="88">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H7" s="88">
         <f>IF(H5=TRUE,(VALUE(H6)),)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I7" s="88">
         <f>IF(I5=TRUE,(VALUE(I6)),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J7" s="88">
         <f>IF(J5=TRUE,(VALUE(J6)),0)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K7" s="105">
         <f>IF(K5=TRUE,(VALUE(K6)),0)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -3859,31 +3858,31 @@
       </c>
       <c r="E9" s="109">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="109">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G9" s="109">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H9" s="109">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I9" s="109">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J9" s="109">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K9" s="110">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L9" s="109"/>
     </row>
@@ -3918,31 +3917,31 @@
       </c>
       <c r="E13" s="88" t="str">
         <f>IF(E9=1," UN MILLONES",IF(E9=2," DOS MILLONES",IF(E9=3," TRES MILLONES",IF(E9=4," CUATRO MILLONES",IF(E9=5," CINCO MILLONES")))))</f>
-        <v xml:space="preserve"> UN MILLONES</v>
-      </c>
-      <c r="F13" s="88" t="str">
+        <v xml:space="preserve"> DOS MILLONES</v>
+      </c>
+      <c r="F13" s="88" t="b">
         <f>IF(F9=1," CIENTO",IF(F9=2," DOSCIENTOS",IF(F9=3," TRESCIENTOS",IF(F9=4," CUATROCIENTOS",IF(F9=5," QUINIENTOS")))))</f>
-        <v xml:space="preserve"> TRESCIENTOS</v>
-      </c>
-      <c r="G13" s="88" t="str">
+        <v>0</v>
+      </c>
+      <c r="G13" s="88" t="b">
         <f>IF(G9=1," DIEZ Y",IF(G9=2," VEINTI",IF(G9=3," TREINTA Y",IF(G9=4," CUARENTA Y",IF(G9=5," CINCUENTA Y")))))</f>
-        <v xml:space="preserve"> CUARENTA Y</v>
+        <v>0</v>
       </c>
       <c r="H13" s="88" t="str">
         <f>IF(H9=1," UN MIL",IF(H9=2," DOS MIL",IF(H9=3," TRES MIL",IF(H9=4," CUATRO MIL",IF(H9=5," CINCO MIL")))))</f>
-        <v xml:space="preserve"> DOS MIL</v>
-      </c>
-      <c r="I13" s="88" t="str">
+        <v xml:space="preserve"> CINCO MIL</v>
+      </c>
+      <c r="I13" s="88" t="b">
         <f>IF(I9=1," CIENTO",IF(I9=2," DOSCIENTOS",IF(I9=3," TRESCIENTOS",IF(I9=4," CUATROCIENTOS",IF(I9=5," QUINIENTOS")))))</f>
-        <v xml:space="preserve"> QUINIENTOS</v>
+        <v>0</v>
       </c>
       <c r="J13" s="88" t="b">
         <f>IF(J9=1," DIEZ Y",IF(J9=2," VEINTI",IF(J9=3," TREINTA Y",IF(J9=4," CUARENTA Y",IF(J9=5," CINCUENTA Y")))))</f>
         <v>0</v>
       </c>
-      <c r="K13" s="105" t="b">
+      <c r="K13" s="105" t="str">
         <f>IF(K9=1," UN",IF(K9=2," DOS",IF(K9=3," TRES",IF(K9=4," CUATRO",IF(K9=5," CINCO")))))</f>
-        <v>0</v>
+        <v xml:space="preserve"> DOS</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -3967,9 +3966,9 @@
         <f>IF(F9=6," SEISCIENTOS",IF(F9=7," SETECIENTOS",IF(F9=8," OCHOCIENTOS",IF(F9=9," NOVECIENTOS"))))</f>
         <v>0</v>
       </c>
-      <c r="G14" s="88" t="b">
+      <c r="G14" s="88" t="str">
         <f>IF(G9=6," SESENTA Y",IF(G9=7," SETENTA Y",IF(G9=8," OCHENTA Y",IF(G9=9," NOVENTA Y"))))</f>
-        <v>0</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="H14" s="88" t="b">
         <f>IF(H9=6," SEIS MIL",IF(H9=7," SIETE MIL",IF(H9=8," OCHO MIL",IF(H9=9," NUEVE MIL"))))</f>
@@ -3981,11 +3980,11 @@
       </c>
       <c r="J14" s="88" t="str">
         <f>IF(J9=6," SESENTA Y",IF(J9=7," SETENTA Y",IF(J9=8," OCHENTA Y",IF(J9=9," NOVENTA Y"))))</f>
-        <v xml:space="preserve"> SETENTA Y</v>
-      </c>
-      <c r="K14" s="105" t="str">
+        <v xml:space="preserve"> SESENTA Y</v>
+      </c>
+      <c r="K14" s="105" t="b">
         <f>IF(K9=6," SEIS",IF(K9=7," SIETE",IF(K9=8," OCHO",IF(K9=9," NUEVE"))))</f>
-        <v xml:space="preserve"> SEIS</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -4004,74 +4003,74 @@
       </c>
       <c r="E15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> UN MILLONES</v>
-      </c>
-      <c r="F15" s="88" t="str">
+        <v xml:space="preserve"> DOS MILLONES</v>
+      </c>
+      <c r="F15" s="88" t="b">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> TRESCIENTOS</v>
+        <v>0</v>
       </c>
       <c r="G15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> CUARENTA Y</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="H15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> DOS MIL</v>
-      </c>
-      <c r="I15" s="88" t="str">
+        <v xml:space="preserve"> CINCO MIL</v>
+      </c>
+      <c r="I15" s="88" t="b">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> QUINIENTOS</v>
+        <v>0</v>
       </c>
       <c r="J15" s="88" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> SETENTA Y</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="K15" s="105" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> SEIS</v>
+        <v xml:space="preserve"> DOS</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="107"/>
       <c r="B16" s="92" t="str">
         <f>CONCATENATE(A9,B9,C9,D9,E9,)</f>
-        <v>0001</v>
+        <v>0002</v>
       </c>
       <c r="C16" s="88" t="str">
         <f>CONCATENATE(C9,D9,E9)</f>
-        <v>001</v>
+        <v>002</v>
       </c>
       <c r="D16" s="88" t="str">
         <f>CONCATENATE(D9,E9)</f>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="E16" s="88" t="str">
         <f>CONCATENATE(D9,E9)</f>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="F16" s="88" t="str">
         <f>CONCATENATE(F9,G9,H9)</f>
-        <v>342</v>
+        <v>065</v>
       </c>
       <c r="G16" s="88" t="str">
         <f>CONCATENATE(G9,H9)</f>
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="H16" s="88" t="str">
         <f>CONCATENATE(G9,H9)</f>
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="I16" s="88" t="str">
         <f>CONCATENATE(I9,J9,K9)</f>
-        <v>576</v>
+        <v>062</v>
       </c>
       <c r="J16" s="88" t="str">
         <f>CONCATENATE(J9,K9)</f>
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="K16" s="105" t="str">
         <f>CONCATENATE(J9,K9)</f>
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -4092,9 +4091,9 @@
         <f>IF(E9=0,"",IF(E16="00","",IF(E16="10","",IF(E16="11","",IF(E16="12","",IF(E16="13","",IF(E16="14","",IF(E16="15",""))))))))</f>
         <v>0</v>
       </c>
-      <c r="F17" s="88" t="b">
+      <c r="F17" s="88" t="str">
         <f>IF(F9=0,"",IF(F16="000","",IF(F16="100"," CIEN MIL" )))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="G17" s="88" t="b">
         <f>IF(G9=0,"",IF(G16="00","",IF(G16="10"," DIEZ MIL",IF(G16="11"," ONCE MIL",IF(G16="12"," DOCE MIL",IF(G16="13"," TRECE MIL",IF(G16="14"," CATORCE MIL",IF(G16="15"," QUINCE MIL"))))))))</f>
@@ -4104,9 +4103,9 @@
         <f>IF(H9=0,"",IF(H16="00","",IF(H16="10","",IF(H16="11","",IF(H16="12","",IF(H16="13","",IF(H16="14","",IF(H16="15",""))))))))</f>
         <v>0</v>
       </c>
-      <c r="I17" s="88" t="b">
+      <c r="I17" s="88" t="str">
         <f>IF(I9=0,"",IF(I16="000","",IF(I16="100"," CIEN" )))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="J17" s="88" t="b">
         <f>IF(J9=0,"",IF(J16="00","",IF(J16="10"," DIEZ",IF(J16="11"," ONCE",IF(J16="12"," DOCE",IF(J16="13"," TRECE",IF(J16="14"," CATORCE",IF(J16="15"," QUINCE"))))))))</f>
@@ -4133,7 +4132,7 @@
       </c>
       <c r="E18" s="88" t="str">
         <f>IF(E17=FALSE,E15,E17)</f>
-        <v xml:space="preserve"> UN MILLONES</v>
+        <v xml:space="preserve"> DOS MILLONES</v>
       </c>
       <c r="F18" s="88" t="b">
         <f>IF(F16="200"," DOSCIENTOS MIL",IF(F16="300"," TRESCIENTOS MIL",IF(F16="400"," CUATROCIENTOS MIL",IF(F16="500"," QUINIENTOS MIL",IF(F16="600"," SEISCIENTOS MIL",IF(F16="700"," SETECIENTOS MIL",IF(F16="800"," OCHOCIENTOS MIL",IF(F16="900"," NOVECIENTOS MIL"))))))))</f>
@@ -4145,11 +4144,11 @@
       </c>
       <c r="H18" s="88" t="str">
         <f>IF(H17=FALSE,H15,H17)</f>
-        <v xml:space="preserve"> DOS MIL</v>
+        <v xml:space="preserve"> CINCO MIL</v>
       </c>
       <c r="I18" s="88" t="str">
         <f>IF(I17=FALSE,I15,I17)</f>
-        <v xml:space="preserve"> QUINIENTOS</v>
+        <v/>
       </c>
       <c r="J18" s="88" t="b">
         <f>IF(J16="20"," VEINTE",IF(J16="30"," TREINTA",IF(J16="40"," CUARENTA",IF(J16="50"," CINCUENTA",IF(J16="60"," SESENTA",IF(J16="80"," OCHENTA",IF(J16="90"," NOVENTA")))))))</f>
@@ -4157,7 +4156,7 @@
       </c>
       <c r="K18" s="105" t="str">
         <f>IF(K17=FALSE,K15,K17)</f>
-        <v xml:space="preserve"> SEIS</v>
+        <v xml:space="preserve"> DOS</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -4173,19 +4172,19 @@
       </c>
       <c r="E19" s="88" t="str">
         <f>CONCATENATE(B9,C9,D9,E9)</f>
-        <v>0001</v>
+        <v>0002</v>
       </c>
       <c r="F19" s="88" t="str">
         <f>IF(F17=FALSE,F15,F17)</f>
-        <v xml:space="preserve"> TRESCIENTOS</v>
+        <v/>
       </c>
       <c r="G19" s="88" t="str">
         <f>IF(G17=FALSE,G15,G17)</f>
-        <v xml:space="preserve"> CUARENTA Y</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="J19" s="88" t="str">
         <f>IF(J17=FALSE,J15,J17)</f>
-        <v xml:space="preserve"> SETENTA Y</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="K19" s="105"/>
     </row>
@@ -4202,19 +4201,19 @@
       </c>
       <c r="E20" s="88" t="str">
         <f>IF(E19="0001","UN MILLÓN",E18)</f>
-        <v>UN MILLÓN</v>
+        <v xml:space="preserve"> DOS MILLONES</v>
       </c>
       <c r="F20" s="88" t="str">
         <f>IF(F18=FALSE,F19,F18)</f>
-        <v xml:space="preserve"> TRESCIENTOS</v>
+        <v/>
       </c>
       <c r="G20" s="88" t="str">
         <f>IF(G18=FALSE,G19,G18)</f>
-        <v xml:space="preserve"> CUARENTA Y</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="J20" s="88" t="str">
         <f>IF(J18=FALSE,J19,J18)</f>
-        <v xml:space="preserve"> SETENTA Y</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="K20" s="105"/>
     </row>
@@ -4239,31 +4238,31 @@
       </c>
       <c r="E22" s="111" t="str">
         <f>E20</f>
-        <v>UN MILLÓN</v>
+        <v xml:space="preserve"> DOS MILLONES</v>
       </c>
       <c r="F22" s="111" t="str">
         <f>F20</f>
-        <v xml:space="preserve"> TRESCIENTOS</v>
+        <v/>
       </c>
       <c r="G22" s="111" t="str">
         <f>G20</f>
-        <v xml:space="preserve"> CUARENTA Y</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="H22" s="111" t="str">
         <f>H18</f>
-        <v xml:space="preserve"> DOS MIL</v>
+        <v xml:space="preserve"> CINCO MIL</v>
       </c>
       <c r="I22" s="111" t="str">
         <f>I18</f>
-        <v xml:space="preserve"> QUINIENTOS</v>
+        <v/>
       </c>
       <c r="J22" s="111" t="str">
         <f>J20</f>
-        <v xml:space="preserve"> SETENTA Y</v>
+        <v xml:space="preserve"> SESENTA Y</v>
       </c>
       <c r="K22" s="112" t="str">
         <f>K18</f>
-        <v xml:space="preserve"> SEIS</v>
+        <v xml:space="preserve"> DOS</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>